<commit_message>
Preparing app for finalization, every log point written on the landing page.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -448,41 +448,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMG_4405.JPG_3clusters.png</t>
+          <t>IMG_4402.JPG_4clusters.png</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28.9120589065744</v>
+        <v>2.749519586250239</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IMG_4402.JPG_4clusters.png</t>
+          <t>IMG_4403.JPG_4clusters.png</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15.64918256055364</v>
+        <v>1.726557732632442</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IMG_4403.JPG_4clusters.png</t>
+          <t>IMG_4399.JPG_4clusters.png</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9.800817384083047</v>
+        <v>2.878927310444024</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IMG_4399.JPG_4clusters.png</t>
+          <t>IMG_4405.JPG_4clusters.png</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16.19130020761246</v>
+        <v>5.092057187419351</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28.14818325259516</v>
+        <v>4.964401783435124</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>34.10930889965399</v>
+        <v>6.01646226207128</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>25.20438876124568</v>
+        <v>4.445653220885297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>